<commit_message>
add the 3x12x3 potato testing data
</commit_message>
<xml_diff>
--- a/data/raw/dr_db.xlsx
+++ b/data/raw/dr_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/Dose_Response/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9F473E-1A72-564F-AE2B-D2E553786EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA644BC-116D-F549-9142-A16A2AA73B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1" xr2:uid="{09121203-F725-7841-956D-4A9953E65086}"/>
+    <workbookView xWindow="2100" yWindow="760" windowWidth="32460" windowHeight="19880" activeTab="1" xr2:uid="{09121203-F725-7841-956D-4A9953E65086}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -290,9 +290,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>Unique ID for every subject in this database, no repeats allowed</t>
-  </si>
-  <si>
     <t>Which studies are already in here?</t>
   </si>
   <si>
@@ -307,12 +304,63 @@
   <si>
     <t xml:space="preserve"> This study is excluded, this isn't DR testing, we won't use it</t>
   </si>
+  <si>
+    <t>Initially we thought this represented unique potatoes. We learned it does not, so it currently means nothing at all.</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>EB-3</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>3x12x3 potato tests_08_02_2024</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>POTATO TESTING AUGUST 2 2024-ryan</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -367,6 +415,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -395,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -415,18 +470,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -523,18 +599,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -608,10 +672,10 @@
     <tableColumn id="8" xr3:uid="{56F928AF-CB3C-E149-8BCB-A51BF644C943}" name="n_uni" dataDxfId="21"/>
     <tableColumn id="9" xr3:uid="{ED7FD3EA-7EC8-C44E-B842-D41BC4E34E28}" name="n_bipolar" dataDxfId="20"/>
     <tableColumn id="10" xr3:uid="{4C58E439-210E-624E-8CBA-1B8E3E20A8D0}" name="n_biphasic" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{33292D2D-93D1-0141-B0C4-17ADAC1EC6C4}" name="n_train_rep" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{06C7383A-C15D-0F42-B5DC-7D691A9E0CFD}" name="depth" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{132A6AB1-07EA-F44C-A2A9-8A6937FEFAA1}" name="diameter" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{0FF87492-98E8-9A4C-9C1E-E98D8E1095A4}" name="generator" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{33292D2D-93D1-0141-B0C4-17ADAC1EC6C4}" name="n_train_rep" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{06C7383A-C15D-0F42-B5DC-7D691A9E0CFD}" name="depth" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{132A6AB1-07EA-F44C-A2A9-8A6937FEFAA1}" name="diameter" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{0FF87492-98E8-9A4C-9C1E-E98D8E1095A4}" name="generator" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{A18459C3-5D4F-CB4B-ACD6-1064E84E0396}" name="experiment_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -619,22 +683,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C29E30DD-FBFD-ED4C-AB59-BD9C1B2C8A3E}" name="Table5" displayName="Table5" ref="A1:O550" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C29E30DD-FBFD-ED4C-AB59-BD9C1B2C8A3E}" name="Table5" displayName="Table5" ref="A1:O550" totalsRowShown="0" headerRowDxfId="18">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{07AA4434-D3EA-904D-9B49-A29B767D968A}" name="id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{60A59FF1-F641-7B4C-84A1-9730C0401CE0}" name="species" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{0020F4F1-3D27-004D-B06E-F766281016D4}" name="lesion_num" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{CAEFC5A6-354E-C247-8CCA-AE70E4009996}" name="application_num" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{BB712484-2619-5E46-9E06-15FAA0A58D62}" name="voltage" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{95534238-E903-0544-9199-5E0678FB44F8}" name="pulse_seq" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{3D36EE62-2338-2D42-90C1-FD561C8DA56B}" name="waveform" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{CF414030-D9BA-0543-9D59-E95A8B559EFD}" name="n_uni" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{0560D0A4-EEA2-DD46-B0D1-B0E8B1859464}" name="n_bipolar" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5CAC8C10-A00F-C744-BBEE-A412EDC09017}" name="n_biphasic" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{E02A03D0-7553-764F-A1EC-C19531AD6694}" name="n_train_rep" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{BC82ECAB-E272-B945-B4F9-404923E69B2C}" name="depth" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{7BC62987-DBF6-8242-9A66-477FF420C321}" name="diameter" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{BA758137-F60F-984E-BB79-AE9C83BFE808}" name="generator" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{07AA4434-D3EA-904D-9B49-A29B767D968A}" name="id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{60A59FF1-F641-7B4C-84A1-9730C0401CE0}" name="species" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{0020F4F1-3D27-004D-B06E-F766281016D4}" name="lesion_num" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{CAEFC5A6-354E-C247-8CCA-AE70E4009996}" name="application_num" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{BB712484-2619-5E46-9E06-15FAA0A58D62}" name="voltage" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{95534238-E903-0544-9199-5E0678FB44F8}" name="pulse_seq" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{3D36EE62-2338-2D42-90C1-FD561C8DA56B}" name="waveform" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{CF414030-D9BA-0543-9D59-E95A8B559EFD}" name="n_uni" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{0560D0A4-EEA2-DD46-B0D1-B0E8B1859464}" name="n_bipolar" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{5CAC8C10-A00F-C744-BBEE-A412EDC09017}" name="n_biphasic" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{E02A03D0-7553-764F-A1EC-C19531AD6694}" name="n_train_rep" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{BC82ECAB-E272-B945-B4F9-404923E69B2C}" name="depth" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{7BC62987-DBF6-8242-9A66-477FF420C321}" name="diameter" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{BA758137-F60F-984E-BB79-AE9C83BFE808}" name="generator" dataDxfId="4"/>
     <tableColumn id="15" xr3:uid="{9B261674-7C1B-1B4B-A054-F208FE92BC4A}" name="experiment_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -988,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56265552-5F8B-5640-AFF4-B9B334353120}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A26" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,87 +1081,87 @@
       <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="F2" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="F3" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="F4" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
       <c r="F5" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
@@ -1217,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
@@ -1399,7 +1463,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -1424,10 +1488,20 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1445,6 +1519,8 @@
     <hyperlink ref="A46" r:id="rId7" display="https://fieldmedical.sharepoint.com/:x:/s/Clinical/EULrYtYXaX9Ko1vMFYDemYUBTHMUr5r933GB3QPXS1uAQQ?e=LeJ9jm" xr:uid="{3AA702AA-FC97-6A4D-B588-4BFDBC3676DD}"/>
     <hyperlink ref="A47" r:id="rId8" display="https://fieldmedical.sharepoint.com/:x:/s/Clinical/ESmePT5OzgBBs2eSIMPqL2kBjzTHwcXzE-HJD6lMbGlWPw?e=cTdXlF" xr:uid="{2611F497-A6DF-574C-986D-6BBEF2230740}"/>
     <hyperlink ref="A48" r:id="rId9" display="https://fieldmedical.sharepoint.com/:x:/s/Clinical/EWJo2dOKUsFEqZp0BE2yh5oB0u1cBdYOLsm1hlDaM7W6wQ?e=cyp6ab" xr:uid="{5509B9D5-BD42-1C4E-BF9A-806DD1643B65}"/>
+    <hyperlink ref="A49" r:id="rId10" xr:uid="{A120493C-69FC-904B-AF0E-A0955CB4ABE0}"/>
+    <hyperlink ref="A50" r:id="rId11" xr:uid="{99DBAF5F-549B-D747-9ADF-C6B0134B02F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1452,21 +1528,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F5BF2D-E5D2-C74E-BDAA-5F5BFA9E62BE}">
-  <dimension ref="A1:W171"/>
+  <dimension ref="A1:W225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C175" sqref="C175"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M216" sqref="M216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="16" customWidth="1"/>
-    <col min="5" max="10" width="10.83203125" style="3"/>
-    <col min="11" max="11" width="11.6640625" style="3" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="6" style="3" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="16" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="3"/>
     <col min="15" max="15" width="13.6640625" customWidth="1"/>
     <col min="18" max="18" width="16.83203125" customWidth="1"/>
   </cols>
@@ -1478,10 +1561,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1554,10 +1637,10 @@
       <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="15">
         <v>13</v>
       </c>
       <c r="O2" t="s">
@@ -1599,10 +1682,10 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="15">
         <v>4.5</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="15">
         <v>16.2</v>
       </c>
       <c r="O3" t="s">
@@ -1643,10 +1726,10 @@
       <c r="K4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="15">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="15">
         <v>16</v>
       </c>
       <c r="O4" t="s">
@@ -1687,10 +1770,10 @@
       <c r="K5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="15">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="15">
         <v>16.2</v>
       </c>
       <c r="O5" t="s">
@@ -1731,10 +1814,10 @@
       <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="15">
         <v>16.600000000000001</v>
       </c>
       <c r="O6" t="s">
@@ -1775,10 +1858,10 @@
       <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="15">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="15">
         <v>17.2</v>
       </c>
       <c r="O7" t="s">
@@ -1819,10 +1902,10 @@
       <c r="K8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="15">
         <v>5.9</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="15">
         <v>18.3</v>
       </c>
       <c r="O8" t="s">
@@ -1863,10 +1946,10 @@
       <c r="K9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="15">
         <v>6.2</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="15">
         <v>18.2</v>
       </c>
       <c r="O9" t="s">
@@ -1907,10 +1990,10 @@
       <c r="K10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="15">
         <v>5.6</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="15">
         <v>19</v>
       </c>
       <c r="O10" t="s">
@@ -1951,10 +2034,10 @@
       <c r="K11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="15">
         <v>5.9</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="15">
         <v>19.7</v>
       </c>
       <c r="O11" t="s">
@@ -1995,10 +2078,10 @@
       <c r="K13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="15">
         <v>4.8</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="15">
         <v>13.1</v>
       </c>
       <c r="O13" t="s">
@@ -2039,10 +2122,10 @@
       <c r="K14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="15">
         <v>5.2</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="15">
         <v>16.7</v>
       </c>
       <c r="O14" t="s">
@@ -2083,10 +2166,10 @@
       <c r="K15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="15">
         <v>4.2</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="15">
         <v>16</v>
       </c>
       <c r="O15" t="s">
@@ -2127,10 +2210,10 @@
       <c r="K16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="15">
         <v>5</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="15">
         <v>16</v>
       </c>
       <c r="O16" t="s">
@@ -2171,10 +2254,10 @@
       <c r="K17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="15">
         <v>5.4</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="15">
         <v>17.5</v>
       </c>
       <c r="O17" t="s">
@@ -2215,10 +2298,10 @@
       <c r="K18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="15">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="15">
         <v>16.399999999999999</v>
       </c>
       <c r="O18" t="s">
@@ -2259,10 +2342,10 @@
       <c r="K19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="15">
         <v>6</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="15">
         <v>19</v>
       </c>
       <c r="O19" t="s">
@@ -2303,10 +2386,10 @@
       <c r="K20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="15">
         <v>6.2</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="15">
         <v>18.8</v>
       </c>
       <c r="O20" t="s">
@@ -2347,10 +2430,10 @@
       <c r="K21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="15">
         <v>5.6</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="15">
         <v>19</v>
       </c>
       <c r="O21" t="s">
@@ -2391,10 +2474,10 @@
       <c r="K22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="15">
         <v>6</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="15">
         <v>19.5</v>
       </c>
       <c r="O22" t="s">
@@ -2435,10 +2518,10 @@
       <c r="K24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="15">
         <v>4</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="15">
         <v>13.6</v>
       </c>
       <c r="O24" t="s">
@@ -2479,10 +2562,10 @@
       <c r="K25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="15">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="15">
         <v>16.7</v>
       </c>
       <c r="O25" t="s">
@@ -2523,10 +2606,10 @@
       <c r="K26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="15">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="15">
         <v>16</v>
       </c>
       <c r="O26" t="s">
@@ -2567,10 +2650,10 @@
       <c r="K27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="15">
         <v>5.8</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27" s="15">
         <v>18</v>
       </c>
       <c r="O27" t="s">
@@ -2611,10 +2694,10 @@
       <c r="K28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="15">
         <v>5.3</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="15">
         <v>17.5</v>
       </c>
       <c r="O28" t="s">
@@ -2655,10 +2738,10 @@
       <c r="K29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="15">
         <v>5.2</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29" s="15">
         <v>16.399999999999999</v>
       </c>
       <c r="O29" t="s">
@@ -2699,10 +2782,10 @@
       <c r="K30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="15">
         <v>6.1</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="15">
         <v>19</v>
       </c>
       <c r="O30" t="s">
@@ -2743,10 +2826,10 @@
       <c r="K31" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="15">
         <v>5.3</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="15">
         <v>18.100000000000001</v>
       </c>
       <c r="O31" t="s">
@@ -2787,10 +2870,10 @@
       <c r="K32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="15">
         <v>6</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="15">
         <v>20</v>
       </c>
       <c r="O32" t="s">
@@ -2831,10 +2914,10 @@
       <c r="K33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="15">
         <v>6</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="15">
         <v>20</v>
       </c>
       <c r="O33" t="s">
@@ -2875,10 +2958,10 @@
       <c r="K35" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="15">
         <v>4</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="15">
         <v>10.9</v>
       </c>
       <c r="O35" t="s">
@@ -2926,10 +3009,10 @@
       <c r="K36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="15">
         <v>3.5</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="15">
         <v>9.8000000000000007</v>
       </c>
       <c r="O36" t="s">
@@ -2977,10 +3060,10 @@
       <c r="K37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="15">
         <v>3.9</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="15">
         <v>10.5</v>
       </c>
       <c r="O37" t="s">
@@ -3028,10 +3111,10 @@
       <c r="K38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="15">
         <v>3.9</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="15">
         <v>10.8</v>
       </c>
       <c r="O38" t="s">
@@ -3079,10 +3162,10 @@
       <c r="K39" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="15">
         <v>3.7</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="15">
         <v>9.3000000000000007</v>
       </c>
       <c r="O39" t="s">
@@ -3130,10 +3213,10 @@
       <c r="K40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="15">
         <v>4.3</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="15">
         <v>11.7</v>
       </c>
       <c r="O40" t="s">
@@ -3181,10 +3264,10 @@
       <c r="K41" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="15">
         <v>3.4</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="15">
         <v>10.3</v>
       </c>
       <c r="O41" t="s">
@@ -3232,10 +3315,10 @@
       <c r="K42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="15">
         <v>4</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="15">
         <v>10.4</v>
       </c>
       <c r="O42" t="s">
@@ -3283,10 +3366,10 @@
       <c r="K43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="15">
         <v>2</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="15">
         <v>7.2</v>
       </c>
       <c r="O43" t="s">
@@ -3334,10 +3417,10 @@
       <c r="K44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="15">
         <v>2.7</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44" s="15">
         <v>20</v>
       </c>
       <c r="O44" t="s">
@@ -3394,10 +3477,10 @@
       <c r="K46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="15">
         <v>4</v>
       </c>
-      <c r="M46" s="4">
+      <c r="M46" s="15">
         <v>10.8</v>
       </c>
       <c r="O46" t="s">
@@ -3445,10 +3528,10 @@
       <c r="K47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47" s="15">
         <v>3.6</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47" s="15">
         <v>10.4</v>
       </c>
       <c r="O47" t="s">
@@ -3496,10 +3579,10 @@
       <c r="K48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="15">
         <v>3.8</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48" s="15">
         <v>10</v>
       </c>
       <c r="O48" t="s">
@@ -3540,10 +3623,10 @@
       <c r="K49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="15">
         <v>3.4</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49" s="15">
         <v>9.6999999999999993</v>
       </c>
       <c r="O49" t="s">
@@ -3584,10 +3667,10 @@
       <c r="K50" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50" s="15">
         <v>3.8</v>
       </c>
-      <c r="M50" s="4">
+      <c r="M50" s="15">
         <v>9.8000000000000007</v>
       </c>
       <c r="O50" t="s">
@@ -3628,10 +3711,10 @@
       <c r="K51" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51" s="15">
         <v>3.4</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51" s="15">
         <v>10.1</v>
       </c>
       <c r="O51" t="s">
@@ -3672,10 +3755,10 @@
       <c r="K52" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="15">
         <v>4</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52" s="15">
         <v>10.3</v>
       </c>
       <c r="O52" t="s">
@@ -3716,10 +3799,10 @@
       <c r="K53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53" s="15">
         <v>3</v>
       </c>
-      <c r="M53" s="4">
+      <c r="M53" s="15">
         <v>9.6</v>
       </c>
       <c r="O53" t="s">
@@ -3760,10 +3843,10 @@
       <c r="K54" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L54" s="15">
         <v>2.1</v>
       </c>
-      <c r="M54" s="4">
+      <c r="M54" s="15">
         <v>6.9</v>
       </c>
       <c r="O54" t="s">
@@ -3804,10 +3887,10 @@
       <c r="K55" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L55" s="4">
+      <c r="L55" s="15">
         <v>3.7</v>
       </c>
-      <c r="M55" s="4">
+      <c r="M55" s="15">
         <v>20</v>
       </c>
       <c r="O55" t="s">
@@ -3848,10 +3931,10 @@
       <c r="K57" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L57" s="15">
         <v>3.9</v>
       </c>
-      <c r="M57" s="4">
+      <c r="M57" s="15">
         <v>9.9</v>
       </c>
       <c r="O57" t="s">
@@ -3892,10 +3975,10 @@
       <c r="K58" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L58" s="4">
+      <c r="L58" s="15">
         <v>3.9</v>
       </c>
-      <c r="M58" s="4">
+      <c r="M58" s="15">
         <v>10</v>
       </c>
       <c r="O58" t="s">
@@ -3936,10 +4019,10 @@
       <c r="K59" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L59" s="4">
+      <c r="L59" s="15">
         <v>3.3</v>
       </c>
-      <c r="M59" s="4">
+      <c r="M59" s="15">
         <v>9.8000000000000007</v>
       </c>
       <c r="O59" t="s">
@@ -3980,10 +4063,10 @@
       <c r="K60" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L60" s="4">
+      <c r="L60" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M60" s="4">
+      <c r="M60" s="15">
         <v>11.8</v>
       </c>
       <c r="O60" t="s">
@@ -4024,10 +4107,10 @@
       <c r="K61" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L61" s="4">
+      <c r="L61" s="15">
         <v>3.4</v>
       </c>
-      <c r="M61" s="4">
+      <c r="M61" s="15">
         <v>9.6</v>
       </c>
       <c r="O61" t="s">
@@ -4068,10 +4151,10 @@
       <c r="K62" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L62" s="4">
+      <c r="L62" s="15">
         <v>4</v>
       </c>
-      <c r="M62" s="4">
+      <c r="M62" s="15">
         <v>11.3</v>
       </c>
       <c r="O62" t="s">
@@ -4112,10 +4195,10 @@
       <c r="K63" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L63" s="4">
+      <c r="L63" s="15">
         <v>2.5</v>
       </c>
-      <c r="M63" s="4">
+      <c r="M63" s="15">
         <v>8.3000000000000007</v>
       </c>
       <c r="O63" t="s">
@@ -4156,10 +4239,10 @@
       <c r="K64" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L64" s="4">
+      <c r="L64" s="15">
         <v>3</v>
       </c>
-      <c r="M64" s="4">
+      <c r="M64" s="15">
         <v>9.3000000000000007</v>
       </c>
       <c r="O64" t="s">
@@ -4200,10 +4283,10 @@
       <c r="K65" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L65" s="4">
+      <c r="L65" s="15">
         <v>2</v>
       </c>
-      <c r="M65" s="4">
+      <c r="M65" s="15">
         <v>6.6</v>
       </c>
       <c r="O65" t="s">
@@ -4244,10 +4327,10 @@
       <c r="K66" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L66" s="4">
+      <c r="L66" s="15">
         <v>3</v>
       </c>
-      <c r="M66" s="4">
+      <c r="M66" s="15">
         <v>16</v>
       </c>
       <c r="O66" t="s">
@@ -4288,10 +4371,10 @@
       <c r="K68" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L68" s="1">
+      <c r="L68" s="23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M68" s="1">
+      <c r="M68" s="23">
         <v>16.75</v>
       </c>
       <c r="O68" t="s">
@@ -4332,10 +4415,10 @@
       <c r="K69" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L69" s="1">
+      <c r="L69" s="23">
         <v>5.85</v>
       </c>
-      <c r="M69" s="1">
+      <c r="M69" s="23">
         <v>17.52</v>
       </c>
       <c r="O69" t="s">
@@ -4376,10 +4459,10 @@
       <c r="K70" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L70" s="1">
+      <c r="L70" s="23">
         <v>6.65</v>
       </c>
-      <c r="M70" s="1">
+      <c r="M70" s="23">
         <v>20.83</v>
       </c>
       <c r="O70" t="s">
@@ -4420,10 +4503,10 @@
       <c r="K71" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L71" s="1">
+      <c r="L71" s="23">
         <v>9.3000000000000007</v>
       </c>
-      <c r="M71" s="1">
+      <c r="M71" s="23">
         <v>22.2</v>
       </c>
       <c r="O71" t="s">
@@ -4464,10 +4547,10 @@
       <c r="K72" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L72" s="1">
+      <c r="L72" s="23">
         <v>8.3000000000000007</v>
       </c>
-      <c r="M72" s="1">
+      <c r="M72" s="23">
         <v>25.1</v>
       </c>
       <c r="O72" t="s">
@@ -4508,10 +4591,10 @@
       <c r="K73" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L73" s="1">
+      <c r="L73" s="23">
         <v>8.4</v>
       </c>
-      <c r="M73" s="1">
+      <c r="M73" s="23">
         <v>22</v>
       </c>
       <c r="O73" t="s">
@@ -4552,10 +4635,10 @@
       <c r="K74" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L74" s="1">
+      <c r="L74" s="23">
         <v>10.6</v>
       </c>
-      <c r="M74" s="1">
+      <c r="M74" s="23">
         <v>24.1</v>
       </c>
       <c r="O74" t="s">
@@ -4596,10 +4679,10 @@
       <c r="K75" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L75" s="1">
+      <c r="L75" s="23">
         <v>10.5</v>
       </c>
-      <c r="M75" s="1">
+      <c r="M75" s="23">
         <v>22.3</v>
       </c>
       <c r="O75" t="s">
@@ -4640,10 +4723,10 @@
       <c r="K76" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L76" s="1">
+      <c r="L76" s="23">
         <v>10.6</v>
       </c>
-      <c r="M76" s="1">
+      <c r="M76" s="23">
         <v>22.5</v>
       </c>
       <c r="O76" t="s">
@@ -4684,10 +4767,10 @@
       <c r="K77" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L77" s="1">
+      <c r="L77" s="23">
         <v>11</v>
       </c>
-      <c r="M77" s="1">
+      <c r="M77" s="23">
         <v>22.7</v>
       </c>
       <c r="O77" t="s">
@@ -4728,10 +4811,10 @@
       <c r="K79" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L79" s="1">
+      <c r="L79" s="23">
         <v>4.8</v>
       </c>
-      <c r="M79" s="1"/>
+      <c r="M79" s="23"/>
       <c r="O79" t="s">
         <v>75</v>
       </c>
@@ -4770,8 +4853,8 @@
       <c r="K80" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
+      <c r="L80" s="23"/>
+      <c r="M80" s="23"/>
       <c r="O80" t="s">
         <v>75</v>
       </c>
@@ -4810,8 +4893,8 @@
       <c r="K81" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
+      <c r="L81" s="23"/>
+      <c r="M81" s="23"/>
       <c r="O81" t="s">
         <v>75</v>
       </c>
@@ -4850,10 +4933,10 @@
       <c r="K82" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L82" s="1">
+      <c r="L82" s="23">
         <v>8.3000000000000007</v>
       </c>
-      <c r="M82" s="1">
+      <c r="M82" s="23">
         <v>21.3</v>
       </c>
       <c r="O82" t="s">
@@ -4894,10 +4977,10 @@
       <c r="K83" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L83" s="1">
+      <c r="L83" s="23">
         <v>7.6</v>
       </c>
-      <c r="M83" s="1">
+      <c r="M83" s="23">
         <v>22.3</v>
       </c>
       <c r="O83" t="s">
@@ -4938,10 +5021,10 @@
       <c r="K84" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L84" s="1">
+      <c r="L84" s="23">
         <v>8.4</v>
       </c>
-      <c r="M84" s="1">
+      <c r="M84" s="23">
         <v>22.4</v>
       </c>
       <c r="O84" t="s">
@@ -4982,10 +5065,10 @@
       <c r="K85" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L85" s="1">
+      <c r="L85" s="23">
         <v>10.6</v>
       </c>
-      <c r="M85" s="1">
+      <c r="M85" s="23">
         <v>23.2</v>
       </c>
       <c r="O85" t="s">
@@ -5026,10 +5109,10 @@
       <c r="K86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L86" s="1">
+      <c r="L86" s="23">
         <v>11.8</v>
       </c>
-      <c r="M86" s="1">
+      <c r="M86" s="23">
         <v>23.3</v>
       </c>
       <c r="O86" t="s">
@@ -5070,10 +5153,10 @@
       <c r="K87" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L87" s="1">
+      <c r="L87" s="23">
         <v>10.8</v>
       </c>
-      <c r="M87" s="1">
+      <c r="M87" s="23">
         <v>23.5</v>
       </c>
       <c r="O87" t="s">
@@ -5114,10 +5197,10 @@
       <c r="K88" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L88" s="1">
+      <c r="L88" s="23">
         <v>10.4</v>
       </c>
-      <c r="M88" s="1">
+      <c r="M88" s="23">
         <v>23.8</v>
       </c>
       <c r="O88" t="s">
@@ -5158,10 +5241,10 @@
       <c r="K90" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L90" s="1">
+      <c r="L90" s="23">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M90" s="1"/>
+      <c r="M90" s="23"/>
       <c r="O90" t="s">
         <v>75</v>
       </c>
@@ -5200,8 +5283,8 @@
       <c r="K91" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="23"/>
       <c r="O91" t="s">
         <v>75</v>
       </c>
@@ -5240,8 +5323,8 @@
       <c r="K92" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
+      <c r="L92" s="23"/>
+      <c r="M92" s="23"/>
       <c r="O92" t="s">
         <v>75</v>
       </c>
@@ -5280,10 +5363,10 @@
       <c r="K93" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L93" s="1">
+      <c r="L93" s="23">
         <v>6.7</v>
       </c>
-      <c r="M93" s="1">
+      <c r="M93" s="23">
         <v>23.5</v>
       </c>
       <c r="O93" t="s">
@@ -5324,10 +5407,10 @@
       <c r="K94" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L94" s="1">
+      <c r="L94" s="23">
         <v>7.8</v>
       </c>
-      <c r="M94" s="1">
+      <c r="M94" s="23">
         <v>23.3</v>
       </c>
       <c r="O94" t="s">
@@ -5368,10 +5451,10 @@
       <c r="K95" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L95" s="1">
+      <c r="L95" s="23">
         <v>9.4</v>
       </c>
-      <c r="M95" s="1">
+      <c r="M95" s="23">
         <v>23.3</v>
       </c>
       <c r="O95" t="s">
@@ -5412,10 +5495,10 @@
       <c r="K96" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L96" s="1">
+      <c r="L96" s="23">
         <v>9.6</v>
       </c>
-      <c r="M96" s="1">
+      <c r="M96" s="23">
         <v>24.8</v>
       </c>
       <c r="O96" t="s">
@@ -5456,10 +5539,10 @@
       <c r="K97" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L97" s="1">
+      <c r="L97" s="23">
         <v>12</v>
       </c>
-      <c r="M97" s="1">
+      <c r="M97" s="23">
         <v>23.3</v>
       </c>
       <c r="O97" t="s">
@@ -5500,10 +5583,10 @@
       <c r="K98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L98" s="1">
+      <c r="L98" s="23">
         <v>9.6</v>
       </c>
-      <c r="M98" s="1">
+      <c r="M98" s="23">
         <v>22.8</v>
       </c>
       <c r="O98" t="s">
@@ -5544,10 +5627,10 @@
       <c r="K99" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L99" s="1">
+      <c r="L99" s="23">
         <v>10.5</v>
       </c>
-      <c r="M99" s="1">
+      <c r="M99" s="23">
         <v>23.2</v>
       </c>
       <c r="O99" t="s">
@@ -5588,10 +5671,10 @@
       <c r="K101" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L101" s="1">
+      <c r="L101" s="23">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M101" s="1">
+      <c r="M101" s="23">
         <v>23.4</v>
       </c>
       <c r="O101" t="s">
@@ -5632,10 +5715,10 @@
       <c r="K102" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L102" s="1">
+      <c r="L102" s="23">
         <v>8.5</v>
       </c>
-      <c r="M102" s="1">
+      <c r="M102" s="23">
         <v>27</v>
       </c>
       <c r="O102" t="s">
@@ -5676,10 +5759,10 @@
       <c r="K103" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L103" s="1">
+      <c r="L103" s="23">
         <v>13.5</v>
       </c>
-      <c r="M103" s="1">
+      <c r="M103" s="23">
         <v>40.299999999999997</v>
       </c>
       <c r="O103" t="s">
@@ -5720,10 +5803,10 @@
       <c r="K104" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L104" s="1">
+      <c r="L104" s="23">
         <v>15.8</v>
       </c>
-      <c r="M104" s="1">
+      <c r="M104" s="23">
         <v>45</v>
       </c>
       <c r="O104" t="s">
@@ -5764,10 +5847,10 @@
       <c r="K105" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L105" s="1">
+      <c r="L105" s="23">
         <v>18.3</v>
       </c>
-      <c r="M105" s="1">
+      <c r="M105" s="23">
         <v>57.9</v>
       </c>
       <c r="O105" t="s">
@@ -5808,10 +5891,10 @@
       <c r="K106" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L106" s="1">
+      <c r="L106" s="23">
         <v>17.7</v>
       </c>
-      <c r="M106" s="1">
+      <c r="M106" s="23">
         <v>56.8</v>
       </c>
       <c r="O106" t="s">
@@ -5852,10 +5935,10 @@
       <c r="K107" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L107" s="1">
+      <c r="L107" s="23">
         <v>15.5</v>
       </c>
-      <c r="M107" s="1">
+      <c r="M107" s="23">
         <v>53.8</v>
       </c>
       <c r="O107" t="s">
@@ -5896,10 +5979,10 @@
       <c r="K108" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L108" s="1">
+      <c r="L108" s="23">
         <v>18.2</v>
       </c>
-      <c r="M108" s="1">
+      <c r="M108" s="23">
         <v>52.7</v>
       </c>
       <c r="O108" t="s">
@@ -5940,10 +6023,10 @@
       <c r="K109" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L109" s="1">
+      <c r="L109" s="23">
         <v>15.5</v>
       </c>
-      <c r="M109" s="1">
+      <c r="M109" s="23">
         <v>51.9</v>
       </c>
       <c r="O109" t="s">
@@ -5984,10 +6067,10 @@
       <c r="K110" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L110" s="1">
+      <c r="L110" s="23">
         <v>18.600000000000001</v>
       </c>
-      <c r="M110" s="1">
+      <c r="M110" s="23">
         <v>54.7</v>
       </c>
       <c r="O110" t="s">
@@ -6028,10 +6111,10 @@
       <c r="K112" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L112" s="1">
+      <c r="L112" s="23">
         <v>8.6999999999999993</v>
       </c>
-      <c r="M112" s="1">
+      <c r="M112" s="23">
         <v>27</v>
       </c>
       <c r="O112" t="s">
@@ -6072,10 +6155,10 @@
       <c r="K113" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L113" s="1">
+      <c r="L113" s="23">
         <v>10.8</v>
       </c>
-      <c r="M113" s="1">
+      <c r="M113" s="23">
         <v>27.3</v>
       </c>
       <c r="O113" t="s">
@@ -6116,10 +6199,10 @@
       <c r="K114" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L114" s="1">
+      <c r="L114" s="23">
         <v>14.3</v>
       </c>
-      <c r="M114" s="1">
+      <c r="M114" s="23">
         <v>37.799999999999997</v>
       </c>
       <c r="O114" t="s">
@@ -6160,10 +6243,10 @@
       <c r="K115" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L115" s="1">
+      <c r="L115" s="23">
         <v>15</v>
       </c>
-      <c r="M115" s="1">
+      <c r="M115" s="23">
         <v>47.9</v>
       </c>
       <c r="O115" t="s">
@@ -6204,10 +6287,10 @@
       <c r="K116" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L116" s="1">
+      <c r="L116" s="23">
         <v>18</v>
       </c>
-      <c r="M116" s="1">
+      <c r="M116" s="23">
         <v>53</v>
       </c>
       <c r="O116" t="s">
@@ -6248,10 +6331,10 @@
       <c r="K117" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L117" s="1">
+      <c r="L117" s="23">
         <v>15.3</v>
       </c>
-      <c r="M117" s="1">
+      <c r="M117" s="23">
         <v>46.8</v>
       </c>
       <c r="O117" t="s">
@@ -6292,10 +6375,10 @@
       <c r="K118" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L118" s="1">
+      <c r="L118" s="23">
         <v>18.399999999999999</v>
       </c>
-      <c r="M118" s="1">
+      <c r="M118" s="23">
         <v>54.7</v>
       </c>
       <c r="O118" t="s">
@@ -6336,10 +6419,10 @@
       <c r="K119" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L119" s="1">
+      <c r="L119" s="23">
         <v>16.399999999999999</v>
       </c>
-      <c r="M119" s="1">
+      <c r="M119" s="23">
         <v>52.1</v>
       </c>
       <c r="O119" t="s">
@@ -6380,10 +6463,10 @@
       <c r="K120" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L120" s="1">
+      <c r="L120" s="23">
         <v>17.5</v>
       </c>
-      <c r="M120" s="1">
+      <c r="M120" s="23">
         <v>53.3</v>
       </c>
       <c r="O120" t="s">
@@ -6424,10 +6507,10 @@
       <c r="K121" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L121" s="1">
+      <c r="L121" s="23">
         <v>17.3</v>
       </c>
-      <c r="M121" s="1">
+      <c r="M121" s="23">
         <v>54.4</v>
       </c>
       <c r="O121" t="s">
@@ -6468,10 +6551,10 @@
       <c r="K123" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L123" s="1">
+      <c r="L123" s="23">
         <v>8.6999999999999993</v>
       </c>
-      <c r="M123" s="1">
+      <c r="M123" s="23">
         <v>23.5</v>
       </c>
       <c r="O123" t="s">
@@ -6512,10 +6595,10 @@
       <c r="K124" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L124" s="1">
+      <c r="L124" s="23">
         <v>14.6</v>
       </c>
-      <c r="M124" s="1">
+      <c r="M124" s="23">
         <v>31</v>
       </c>
       <c r="O124" t="s">
@@ -6556,10 +6639,10 @@
       <c r="K125" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L125" s="1">
+      <c r="L125" s="23">
         <v>14.8</v>
       </c>
-      <c r="M125" s="1">
+      <c r="M125" s="23">
         <v>44.5</v>
       </c>
       <c r="O125" t="s">
@@ -6600,10 +6683,10 @@
       <c r="K126" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L126" s="1">
+      <c r="L126" s="23">
         <v>16.8</v>
       </c>
-      <c r="M126" s="1">
+      <c r="M126" s="23">
         <v>47</v>
       </c>
       <c r="O126" t="s">
@@ -6644,10 +6727,10 @@
       <c r="K127" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L127" s="1">
+      <c r="L127" s="23">
         <v>15.8</v>
       </c>
-      <c r="M127" s="1">
+      <c r="M127" s="23">
         <v>57.5</v>
       </c>
       <c r="O127" t="s">
@@ -6688,10 +6771,10 @@
       <c r="K128" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L128" s="1">
+      <c r="L128" s="23">
         <v>15.8</v>
       </c>
-      <c r="M128" s="1">
+      <c r="M128" s="23">
         <v>57.9</v>
       </c>
       <c r="O128" t="s">
@@ -6732,10 +6815,10 @@
       <c r="K129" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L129" s="1">
+      <c r="L129" s="23">
         <v>18</v>
       </c>
-      <c r="M129" s="1">
+      <c r="M129" s="23">
         <v>50.4</v>
       </c>
       <c r="O129" t="s">
@@ -6776,10 +6859,10 @@
       <c r="K130" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L130" s="1">
+      <c r="L130" s="23">
         <v>15.7</v>
       </c>
-      <c r="M130" s="1">
+      <c r="M130" s="23">
         <v>53.1</v>
       </c>
       <c r="O130" t="s">
@@ -6820,10 +6903,10 @@
       <c r="K131" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L131" s="1">
+      <c r="L131" s="23">
         <v>14.9</v>
       </c>
-      <c r="M131" s="1">
+      <c r="M131" s="23">
         <v>53.6</v>
       </c>
       <c r="O131" t="s">
@@ -6864,10 +6947,10 @@
       <c r="K132" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L132" s="1">
+      <c r="L132" s="23">
         <v>18.5</v>
       </c>
-      <c r="M132" s="1">
+      <c r="M132" s="23">
         <v>52.6</v>
       </c>
       <c r="O132" t="s">
@@ -6908,10 +6991,10 @@
       <c r="K134" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L134" s="4">
+      <c r="L134" s="15">
         <v>9</v>
       </c>
-      <c r="M134" s="4">
+      <c r="M134" s="15">
         <v>26</v>
       </c>
       <c r="O134" t="s">
@@ -6952,10 +7035,10 @@
       <c r="K135" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L135" s="4">
+      <c r="L135" s="15">
         <v>10.8</v>
       </c>
-      <c r="M135" s="4">
+      <c r="M135" s="15">
         <v>29</v>
       </c>
       <c r="O135" t="s">
@@ -6996,10 +7079,10 @@
       <c r="K136" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L136" s="4">
+      <c r="L136" s="15">
         <v>9</v>
       </c>
-      <c r="M136" s="4">
+      <c r="M136" s="15">
         <v>29</v>
       </c>
       <c r="O136" t="s">
@@ -7040,10 +7123,10 @@
       <c r="K137" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L137" s="4">
+      <c r="L137" s="15">
         <v>18</v>
       </c>
-      <c r="M137" s="4">
+      <c r="M137" s="15">
         <v>40</v>
       </c>
       <c r="O137" t="s">
@@ -7084,10 +7167,10 @@
       <c r="K138" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L138" s="4">
+      <c r="L138" s="15">
         <v>13.5</v>
       </c>
-      <c r="M138" s="4">
+      <c r="M138" s="15">
         <v>40</v>
       </c>
       <c r="O138" t="s">
@@ -7128,10 +7211,10 @@
       <c r="K139" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L139" s="4">
+      <c r="L139" s="15">
         <v>16</v>
       </c>
-      <c r="M139" s="4">
+      <c r="M139" s="15">
         <v>41</v>
       </c>
       <c r="O139" t="s">
@@ -7172,10 +7255,10 @@
       <c r="K140" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L140" s="4">
+      <c r="L140" s="15">
         <v>17</v>
       </c>
-      <c r="M140" s="4">
+      <c r="M140" s="15">
         <v>44</v>
       </c>
       <c r="O140" t="s">
@@ -7216,10 +7299,10 @@
       <c r="K141" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L141" s="4">
+      <c r="L141" s="15">
         <v>21</v>
       </c>
-      <c r="M141" s="4">
+      <c r="M141" s="15">
         <v>42</v>
       </c>
       <c r="O141" t="s">
@@ -7260,10 +7343,10 @@
       <c r="K142" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L142" s="4">
+      <c r="L142" s="15">
         <v>21</v>
       </c>
-      <c r="M142" s="4">
+      <c r="M142" s="15">
         <v>43</v>
       </c>
       <c r="O142" t="s">
@@ -7304,10 +7387,10 @@
       <c r="K143" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L143" s="4">
-        <v>24</v>
-      </c>
-      <c r="M143" s="4">
+      <c r="L143" s="15">
+        <v>24</v>
+      </c>
+      <c r="M143" s="15">
         <v>49</v>
       </c>
       <c r="O143" t="s">
@@ -7348,10 +7431,10 @@
       <c r="K145" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L145" s="4">
+      <c r="L145" s="15">
         <v>8.4</v>
       </c>
-      <c r="M145" s="4">
+      <c r="M145" s="15">
         <v>26</v>
       </c>
       <c r="O145" t="s">
@@ -7392,10 +7475,10 @@
       <c r="K146" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L146" s="4">
+      <c r="L146" s="15">
         <v>13</v>
       </c>
-      <c r="M146" s="4">
+      <c r="M146" s="15">
         <v>31</v>
       </c>
       <c r="O146" t="s">
@@ -7436,10 +7519,10 @@
       <c r="K147" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L147" s="4">
+      <c r="L147" s="15">
         <v>12.9</v>
       </c>
-      <c r="M147" s="4">
+      <c r="M147" s="15">
         <v>31</v>
       </c>
       <c r="O147" t="s">
@@ -7480,10 +7563,10 @@
       <c r="K148" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L148" s="4">
+      <c r="L148" s="15">
         <v>16</v>
       </c>
-      <c r="M148" s="4">
+      <c r="M148" s="15">
         <v>41</v>
       </c>
       <c r="O148" t="s">
@@ -7524,10 +7607,10 @@
       <c r="K149" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L149" s="4">
+      <c r="L149" s="15">
         <v>15</v>
       </c>
-      <c r="M149" s="4">
+      <c r="M149" s="15">
         <v>43</v>
       </c>
       <c r="O149" t="s">
@@ -7568,10 +7651,10 @@
       <c r="K150" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L150" s="4">
+      <c r="L150" s="15">
         <v>18</v>
       </c>
-      <c r="M150" s="4">
+      <c r="M150" s="15">
         <v>48</v>
       </c>
       <c r="O150" t="s">
@@ -7612,10 +7695,10 @@
       <c r="K151" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L151" s="4">
+      <c r="L151" s="15">
         <v>21</v>
       </c>
-      <c r="M151" s="4">
+      <c r="M151" s="15">
         <v>42</v>
       </c>
       <c r="O151" t="s">
@@ -7656,10 +7739,10 @@
       <c r="K152" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L152" s="4">
+      <c r="L152" s="15">
         <v>21</v>
       </c>
-      <c r="M152" s="4">
+      <c r="M152" s="15">
         <v>49</v>
       </c>
       <c r="O152" t="s">
@@ -7700,10 +7783,10 @@
       <c r="K153" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L153" s="4">
+      <c r="L153" s="15">
         <v>21</v>
       </c>
-      <c r="M153" s="4">
+      <c r="M153" s="15">
         <v>45</v>
       </c>
       <c r="O153" t="s">
@@ -7744,10 +7827,10 @@
       <c r="K154" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L154" s="4">
+      <c r="L154" s="15">
         <v>21</v>
       </c>
-      <c r="M154" s="4">
+      <c r="M154" s="15">
         <v>48</v>
       </c>
       <c r="O154" t="s">
@@ -7788,10 +7871,10 @@
       <c r="K156" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L156" s="4">
+      <c r="L156" s="15">
         <v>8</v>
       </c>
-      <c r="M156" s="4">
+      <c r="M156" s="15">
         <v>27</v>
       </c>
       <c r="O156" t="s">
@@ -7832,10 +7915,10 @@
       <c r="K157" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L157" s="4">
+      <c r="L157" s="15">
         <v>11.4</v>
       </c>
-      <c r="M157" s="4">
+      <c r="M157" s="15">
         <v>29</v>
       </c>
       <c r="O157" t="s">
@@ -7876,10 +7959,10 @@
       <c r="K158" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L158" s="4">
+      <c r="L158" s="15">
         <v>15</v>
       </c>
-      <c r="M158" s="4">
+      <c r="M158" s="15">
         <v>40</v>
       </c>
       <c r="O158" t="s">
@@ -7920,10 +8003,10 @@
       <c r="K159" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L159" s="4">
+      <c r="L159" s="15">
         <v>13</v>
       </c>
-      <c r="M159" s="4">
+      <c r="M159" s="15">
         <v>43</v>
       </c>
       <c r="O159" t="s">
@@ -7964,10 +8047,10 @@
       <c r="K160" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L160" s="4">
+      <c r="L160" s="15">
         <v>14</v>
       </c>
-      <c r="M160" s="4">
+      <c r="M160" s="15">
         <v>41</v>
       </c>
       <c r="O160" t="s">
@@ -8008,10 +8091,10 @@
       <c r="K161" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L161" s="4">
+      <c r="L161" s="15">
         <v>16</v>
       </c>
-      <c r="M161" s="4">
+      <c r="M161" s="15">
         <v>41</v>
       </c>
       <c r="O161" t="s">
@@ -8052,10 +8135,10 @@
       <c r="K162" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L162" s="4">
+      <c r="L162" s="15">
         <v>20</v>
       </c>
-      <c r="M162" s="4">
+      <c r="M162" s="15">
         <v>38</v>
       </c>
       <c r="O162" t="s">
@@ -8096,10 +8179,10 @@
       <c r="K163" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L163" s="4">
+      <c r="L163" s="15">
         <v>23</v>
       </c>
-      <c r="M163" s="4">
+      <c r="M163" s="15">
         <v>45</v>
       </c>
       <c r="O163" t="s">
@@ -8140,10 +8223,10 @@
       <c r="K164" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L164" s="4">
+      <c r="L164" s="15">
         <v>20.7</v>
       </c>
-      <c r="M164" s="4">
+      <c r="M164" s="15">
         <v>48</v>
       </c>
       <c r="O164" t="s">
@@ -8184,10 +8267,10 @@
       <c r="K165" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L165" s="4">
+      <c r="L165" s="15">
         <v>20.399999999999999</v>
       </c>
-      <c r="M165" s="4">
+      <c r="M165" s="15">
         <v>49</v>
       </c>
       <c r="O165" t="s">
@@ -8195,19 +8278,2267 @@
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D167"/>
-      <c r="L167" s="4"/>
-      <c r="M167" s="4"/>
+      <c r="A167" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D167" s="15">
+        <v>1</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J167" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K167" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L167" s="16">
+        <v>7</v>
+      </c>
+      <c r="M167" s="16">
+        <v>35</v>
+      </c>
+      <c r="N167" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O167" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D168" s="15">
+        <v>2</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J168" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K168" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L168" s="16">
+        <v>12</v>
+      </c>
+      <c r="M168" s="16">
+        <v>42</v>
+      </c>
+      <c r="N168" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O168" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D169"/>
+      <c r="A169" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D169" s="15">
+        <v>3</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I169" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J169" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K169" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L169" s="16">
+        <v>13</v>
+      </c>
+      <c r="M169" s="16">
+        <v>43</v>
+      </c>
+      <c r="N169" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O169" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D170" s="15">
+        <v>4</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J170" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K170" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L170" s="16">
+        <v>12</v>
+      </c>
+      <c r="M170" s="16">
+        <v>41</v>
+      </c>
+      <c r="N170" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O170" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D171"/>
+      <c r="A171" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="15">
+        <v>5</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I171" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J171" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K171" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L171" s="16">
+        <v>14</v>
+      </c>
+      <c r="M171" s="16">
+        <v>40</v>
+      </c>
+      <c r="N171" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O171" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D172" s="15">
+        <v>6</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L172" s="16">
+        <v>14</v>
+      </c>
+      <c r="M172" s="16">
+        <v>42</v>
+      </c>
+      <c r="N172" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O172" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D173" s="15">
+        <v>7</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K173" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L173" s="16">
+        <v>14</v>
+      </c>
+      <c r="M173" s="16">
+        <v>45</v>
+      </c>
+      <c r="N173" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O173" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D174" s="15">
+        <v>8</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J174" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K174" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L174" s="16">
+        <v>14</v>
+      </c>
+      <c r="M174" s="16">
+        <v>46</v>
+      </c>
+      <c r="N174" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O174" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175" s="15">
+        <v>9</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J175" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K175" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L175" s="16">
+        <v>15</v>
+      </c>
+      <c r="M175" s="16">
+        <v>46</v>
+      </c>
+      <c r="N175" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O175" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D176" s="15">
+        <v>10</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J176" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L176" s="16">
+        <v>14</v>
+      </c>
+      <c r="M176" s="16">
+        <v>45</v>
+      </c>
+      <c r="N176" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O176" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D178" s="15">
+        <v>1</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J178" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K178" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L178" s="16">
+        <v>7</v>
+      </c>
+      <c r="M178" s="16">
+        <v>34</v>
+      </c>
+      <c r="N178" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O178" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A179" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D179" s="15">
+        <v>2</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H179" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K179" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L179" s="16">
+        <v>11</v>
+      </c>
+      <c r="M179" s="16">
+        <v>37</v>
+      </c>
+      <c r="N179" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O179" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A180" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D180" s="15">
+        <v>3</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K180" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L180" s="16">
+        <v>12</v>
+      </c>
+      <c r="M180" s="16">
+        <v>42</v>
+      </c>
+      <c r="N180" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O180" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A181" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D181" s="15">
+        <v>4</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H181" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I181" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J181" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K181" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L181" s="16">
+        <v>13</v>
+      </c>
+      <c r="M181" s="16">
+        <v>42</v>
+      </c>
+      <c r="N181" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O181" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A182" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D182" s="15">
+        <v>5</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H182" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I182" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J182" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K182" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L182" s="16">
+        <v>14</v>
+      </c>
+      <c r="M182" s="16">
+        <v>43</v>
+      </c>
+      <c r="N182" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O182" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A183" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D183" s="15">
+        <v>6</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H183" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I183" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J183" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K183" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L183" s="16">
+        <v>14</v>
+      </c>
+      <c r="M183" s="16">
+        <v>43</v>
+      </c>
+      <c r="N183" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O183" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A184" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D184" s="15">
+        <v>7</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H184" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I184" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J184" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K184" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L184" s="16">
+        <v>14</v>
+      </c>
+      <c r="M184" s="16">
+        <v>45</v>
+      </c>
+      <c r="N184" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O184" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A185" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D185" s="15">
+        <v>8</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H185" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I185" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J185" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K185" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L185" s="16">
+        <v>14</v>
+      </c>
+      <c r="M185" s="16">
+        <v>44</v>
+      </c>
+      <c r="N185" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O185" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A186" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D186" s="15">
+        <v>9</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I186" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J186" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K186" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L186" s="16">
+        <v>14</v>
+      </c>
+      <c r="M186" s="16">
+        <v>46</v>
+      </c>
+      <c r="N186" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O186" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A187" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187" s="15">
+        <v>10</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H187" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J187" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K187" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L187" s="16">
+        <v>14</v>
+      </c>
+      <c r="M187" s="16">
+        <v>45</v>
+      </c>
+      <c r="N187" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O187" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A189" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D189" s="15">
+        <v>1</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H189" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J189" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K189" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L189" s="16">
+        <v>8</v>
+      </c>
+      <c r="M189" s="16">
+        <v>35</v>
+      </c>
+      <c r="N189" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O189" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A190" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D190" s="15">
+        <v>2</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H190" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I190" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J190" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K190" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L190" s="16">
+        <v>13</v>
+      </c>
+      <c r="M190" s="16">
+        <v>40</v>
+      </c>
+      <c r="N190" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O190" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A191" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D191" s="15">
+        <v>3</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H191" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I191" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J191" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K191" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L191" s="16">
+        <v>13</v>
+      </c>
+      <c r="M191" s="16">
+        <v>41</v>
+      </c>
+      <c r="N191" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O191" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A192" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D192" s="15">
+        <v>4</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H192" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I192" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J192" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K192" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L192" s="16">
+        <v>12</v>
+      </c>
+      <c r="M192" s="16">
+        <v>40</v>
+      </c>
+      <c r="N192" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O192" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A193" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D193" s="15">
+        <v>5</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H193" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I193" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J193" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K193" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L193" s="16">
+        <v>14</v>
+      </c>
+      <c r="M193" s="16">
+        <v>44</v>
+      </c>
+      <c r="N193" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O193" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A194" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D194" s="15">
+        <v>6</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H194" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I194" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J194" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K194" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L194" s="16">
+        <v>14</v>
+      </c>
+      <c r="M194" s="16">
+        <v>45</v>
+      </c>
+      <c r="N194" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O194" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D195" s="15">
+        <v>7</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H195" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I195" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J195" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K195" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L195" s="16">
+        <v>14</v>
+      </c>
+      <c r="M195" s="16">
+        <v>45</v>
+      </c>
+      <c r="N195" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O195" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D196" s="15">
+        <v>8</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H196" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I196" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J196" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K196" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L196" s="16">
+        <v>14</v>
+      </c>
+      <c r="M196" s="16">
+        <v>45</v>
+      </c>
+      <c r="N196" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O196" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A197" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D197" s="15">
+        <v>9</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H197" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I197" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J197" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K197" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L197" s="16">
+        <v>14</v>
+      </c>
+      <c r="M197" s="16">
+        <v>44</v>
+      </c>
+      <c r="N197" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O197" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D198" s="15">
+        <v>10</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F198" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H198" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I198" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J198" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K198" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L198" s="16">
+        <v>15</v>
+      </c>
+      <c r="M198" s="16">
+        <v>45</v>
+      </c>
+      <c r="N198" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O198" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A200" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D200" s="15">
+        <v>1</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H200" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I200" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J200" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K200" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L200" s="16">
+        <v>7</v>
+      </c>
+      <c r="M200" s="16">
+        <v>36</v>
+      </c>
+      <c r="N200" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O200" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A201" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D201" s="15">
+        <v>2</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H201" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I201" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J201" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K201" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L201" s="16">
+        <v>12</v>
+      </c>
+      <c r="M201" s="16">
+        <v>40</v>
+      </c>
+      <c r="N201" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O201" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A202" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D202" s="15">
+        <v>3</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H202" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I202" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J202" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K202" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L202" s="16">
+        <v>13</v>
+      </c>
+      <c r="M202" s="16">
+        <v>40</v>
+      </c>
+      <c r="N202" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O202" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A203" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D203" s="15">
+        <v>4</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H203" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I203" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K203" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L203" s="16">
+        <v>13</v>
+      </c>
+      <c r="M203" s="16">
+        <v>42</v>
+      </c>
+      <c r="N203" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O203" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A204" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D204" s="15">
+        <v>5</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H204" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I204" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J204" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K204" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L204" s="16">
+        <v>13</v>
+      </c>
+      <c r="M204" s="16">
+        <v>42</v>
+      </c>
+      <c r="N204" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O204" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A205" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D205" s="15">
+        <v>6</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H205" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I205" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J205" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K205" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L205" s="16">
+        <v>15</v>
+      </c>
+      <c r="M205" s="16">
+        <v>45</v>
+      </c>
+      <c r="N205" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O205" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A206" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D206" s="15">
+        <v>7</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H206" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I206" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J206" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L206" s="16">
+        <v>14</v>
+      </c>
+      <c r="M206" s="16">
+        <v>45</v>
+      </c>
+      <c r="N206" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O206" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A207" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D207" s="15">
+        <v>8</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H207" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J207" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K207" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L207" s="16">
+        <v>14</v>
+      </c>
+      <c r="M207" s="16">
+        <v>45</v>
+      </c>
+      <c r="N207" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O207" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A208" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D208" s="15">
+        <v>9</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H208" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I208" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J208" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K208" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L208" s="16">
+        <v>14</v>
+      </c>
+      <c r="M208" s="16">
+        <v>44</v>
+      </c>
+      <c r="N208" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O208" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A209" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D209" s="15">
+        <v>10</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H209" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I209" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J209" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K209" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L209" s="16">
+        <v>14</v>
+      </c>
+      <c r="M209" s="16">
+        <v>46</v>
+      </c>
+      <c r="N209" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O209" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A211" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D211" s="16">
+        <v>5</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F211" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H211" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L211" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="M211" s="24">
+        <v>55</v>
+      </c>
+      <c r="N211" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O211" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A213" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D213" s="16">
+        <v>5</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H213" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J213" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K213" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L213" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="M213" s="24">
+        <v>50</v>
+      </c>
+      <c r="N213" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O213" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A215" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B215" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C215" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D215" s="19">
+        <v>5</v>
+      </c>
+      <c r="E215" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F215" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G215" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H215" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I215" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J215" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K215" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L215" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M215" s="25">
+        <v>40</v>
+      </c>
+      <c r="N215" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="O215" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A217" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B217" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C217" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D217" s="19">
+        <v>5</v>
+      </c>
+      <c r="E217" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F217" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G217" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H217" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I217" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J217" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K217" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L217" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="M217" s="25">
+        <v>40</v>
+      </c>
+      <c r="N217" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="O217" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A219" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D219" s="16">
+        <v>5</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H219" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I219" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J219" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K219" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L219" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="M219" s="24">
+        <v>55</v>
+      </c>
+      <c r="N219" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O219" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A221" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D221" s="16">
+        <v>5</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H221" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I221" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J221" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K221" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L221" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="M221" s="24">
+        <v>50</v>
+      </c>
+      <c r="N221" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O221" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A223" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D223" s="16">
+        <v>5</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G223" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H223" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I223" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J223" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K223" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L223" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M223" s="24">
+        <v>40</v>
+      </c>
+      <c r="N223" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O223" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A225" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D225" s="16">
+        <v>5</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H225" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I225" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J225" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K225" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L225" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="M225" s="24">
+        <v>40</v>
+      </c>
+      <c r="N225" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O225" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="I174" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -8218,7 +10549,7 @@
           <x14:formula1>
             <xm:f>'Data Validation'!$B$13:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>B1:B214 B216 B218:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="Seems like you selected an unlisted waveform, did you make a typo or do we need to expand the list?" promptTitle="Choose the Pulse Sequence " xr:uid="{686B3C70-6FC7-404A-8B44-E01A73EB6FA6}">
           <x14:formula1>
@@ -8230,13 +10561,13 @@
           <x14:formula1>
             <xm:f>'Data Validation'!$D$4:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G35:G66 G90:G99 G68:G77 G79:G88 F2:F1048576</xm:sqref>
+          <xm:sqref>G35:G66 G90:G99 G68:G77 G79:G88 F2:F214 F216 F218:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="Seems like you selected an unlisted waveform, did you make a typo or do we need to expand the list?" promptTitle="Select Waveform" xr:uid="{82DB6A83-068A-FD41-A020-75D156C5BCB7}">
           <x14:formula1>
             <xm:f>'Data Validation'!$B$4:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G34 G67 G78 G89 G100:G1048576</xm:sqref>
+          <xm:sqref>G1:G34 G67 G78 G89 G100:G214 G216 G218:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8417,12 +10748,12 @@
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
correct typo in raw db
</commit_message>
<xml_diff>
--- a/data/raw/dr_db.xlsx
+++ b/data/raw/dr_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/Dose_Response/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE862133-F911-1241-88C3-0D0015C85B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8733195D-1B2D-4741-BED8-3D6EEA21C362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{09121203-F725-7841-956D-4A9953E65086}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="2" xr2:uid="{09121203-F725-7841-956D-4A9953E65086}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3074" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3076" uniqueCount="135">
   <si>
     <t>id</t>
   </si>
@@ -598,13 +598,13 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1119,74 +1119,74 @@
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
@@ -1421,7 +1421,7 @@
       <c r="P31" s="11"/>
     </row>
     <row r="33" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="9"/>
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="27" t="s">
         <v>124</v>
       </c>
     </row>
@@ -12367,7 +12367,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12991,13 +12991,18 @@
       <c r="L13" t="s">
         <v>6</v>
       </c>
+      <c r="M13">
+        <v>2.75</v>
+      </c>
       <c r="N13" s="14" t="s">
         <v>119</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="Q13" t="s">
         <v>115</v>
       </c>
@@ -13039,13 +13044,18 @@
       <c r="L14" t="s">
         <v>6</v>
       </c>
+      <c r="M14">
+        <v>5.46</v>
+      </c>
       <c r="N14" t="s">
         <v>119</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="P14" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="Q14" t="s">
         <v>115</v>
       </c>
@@ -14014,7 +14024,7 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>10</v>
@@ -14067,7 +14077,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38">
         <v>10</v>
@@ -14120,7 +14130,7 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39">
         <v>10</v>
@@ -14173,7 +14183,7 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -14226,7 +14236,7 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -14276,7 +14286,7 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -14326,7 +14336,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -14379,7 +14389,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45">
         <v>10</v>
@@ -14432,7 +14442,7 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -14485,7 +14495,7 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E47">
         <v>10</v>
@@ -14538,7 +14548,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48">
         <v>10</v>
@@ -14588,7 +14598,7 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E49">
         <v>10</v>

</xml_diff>